<commit_message>
[FIX] 【upgrade to 0.1.2】 fix uncorrent content2list, fix uncorrent ant2c7n, fix latest menu and init excel
</commit_message>
<xml_diff>
--- a/src/main/resources/script/front/micro-service-init-data.xlsx
+++ b/src/main/resources/script/front/micro-service-init-data.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>/iam/task-detail</t>
+          <t>/asgard/task-detail</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>/iam/execution-record</t>
+          <t>/asgard/execution-record</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>/iam/executable-program</t>
+          <t>/asgard/executable-program</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>/iam/saga</t>
+          <t>/asgard/saga</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>/iam/saga-instance</t>
+          <t>/asgard/saga-instance</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>/iam/saga</t>
+          <t>/asgard/saga</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>/iam/saga-instance</t>
+          <t>/asgard/saga-instance</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>/iam/saga-instance</t>
+          <t>/asgard/saga-instance</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>/iam/task-detail</t>
+          <t>/asgard/task-detail</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>/iam/execution-record</t>
+          <t>/asgard/execution-record</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>/iam/executable-program</t>
+          <t>/asgard/executable-program</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -930,7 +930,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>/iam/saga-instance</t>
+          <t>/asgard/saga-instance</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>/iam/task-detail</t>
+          <t>/asgard/task-detail</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>/iam/execution-record</t>
+          <t>/asgard/execution-record</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>/iam/executable-program</t>
+          <t>/asgard/executable-program</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">

</xml_diff>